<commit_message>
Update TITAN project with fully working pipeline
</commit_message>
<xml_diff>
--- a/outputs/titan_tips.xlsx
+++ b/outputs/titan_tips.xlsx
@@ -480,7 +480,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Dolphins</t>
+          <t>Roosters</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Knights</t>
+          <t>Rabbitohs</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Dragons</t>
+          <t>Wests Tigers</t>
         </is>
       </c>
     </row>
@@ -565,7 +565,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Broncos</t>
+          <t>Panthers</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Raiders</t>
+          <t>Storm</t>
         </is>
       </c>
     </row>

</xml_diff>